<commit_message>
[done v1 Tiktok với khoảng 20 videos - tuy nhiên Scripts đang 1 Role]up file được merge khi xài tới 4 acc API TIKTOK
https://docs.google.com/spreadsheets/d/1OSXwct4aiIA_r-MTW4yZjPSzYKTAM0IQ/edit?usp=sharing&ouid=106070054805248205712&rtpof=true&sd=true

----
Bài Crawl Moxie

Em gửi phần TikTok trước.
- Tiktok	Với gói Free: khoảng 10 videos/ngày, hiện auto tầm 90% với gói free.
(Gói có phí thì auto: 100% ).
- Transcriptions thì đang chưa có phân vai 2 người (chỉ có transcriptions thuần ạ).
-------
======
gói free đảo qua các account khác nhau
</commit_message>
<xml_diff>
--- a/Crawl_Tiktok/tiktok2download/excel_output/MoxieRobot_Videos.xlsx
+++ b/Crawl_Tiktok/tiktok2download/excel_output/MoxieRobot_Videos.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/BasicTasks_PreProcessingTools/Crawl_Tiktok/tiktok2download/excel_output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3FA522FF9473899742BFB53C196E039379798E19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC9FA125-A13D-435F-A9F5-D048432DBD1C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Video ID</t>
   </si>
@@ -58,15 +64,6 @@
     <t>Transcriptions</t>
   </si>
   <si>
-    <t>id7379788763544833310</t>
-  </si>
-  <si>
-    <t>id7379056557100731679</t>
-  </si>
-  <si>
-    <t>id7377188889095703851</t>
-  </si>
-  <si>
     <t>id7376446618729483562</t>
   </si>
   <si>
@@ -112,15 +109,6 @@
     <t>id7353810628466822442</t>
   </si>
   <si>
-    <t>Thank you to all the teachers who make learning a fun and exciting experience! #teacherapprecationweek #moxierobot #socialemotionaldevelopment #playbasedlearning</t>
-  </si>
-  <si>
-    <t>Did you know Moxie comes with a built-in KidFilter™️ ? When kids start saying things or asking questions that are outside Moxie’s wheelhouse, she will recommend that they talk to a trusted adult! This way Moxie can focus on improving their social-emotional skills and allow parents and guardians to have discussions with their kids. #moxierobot #socialemotionaldevelopment #playbasedlearning #robotsontiktok</t>
-  </si>
-  <si>
-    <t>It’s because they’re a real tough kid 😉 🤖 #moxierobot #socialemotionaldevelopment #playbasedlearning</t>
-  </si>
-  <si>
     <t>Moxie is giving steampunk. #moxierobot #fallout</t>
   </si>
   <si>
@@ -166,15 +154,6 @@
     <t>Don’t worry, Moxie comes programmed with dozens of games and activities! 🤖 #moxierobot #socialemotionaldevelopment #playbasedlearning #robotsontiktok</t>
   </si>
   <si>
-    <t>https://www.tiktok.com/@moxierobot/video/7379788763544833310</t>
-  </si>
-  <si>
-    <t>https://www.tiktok.com/@moxierobot/video/7379056557100731679</t>
-  </si>
-  <si>
-    <t>https://www.tiktok.com/@moxierobot/video/7377188889095703851</t>
-  </si>
-  <si>
     <t>https://www.tiktok.com/@moxierobot/video/7376446618729483562</t>
   </si>
   <si>
@@ -220,15 +199,6 @@
     <t>https://www.tiktok.com/@moxierobot/video/7353810628466822442</t>
   </si>
   <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oIxHQmFPf9VdZjwqEgDAIbajR1mARBhEEkEBfG/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=1086&amp;bt=543&amp;cs=0&amp;ds=3&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=ZjVmM2YzZmk4PDpmNTVlZUBpams1aWs5cnE3czMzaTczNEBhYWBeYjYuNi8xNWAyXy8uYSNtNGhxMmRjYWlgLS1kMTJzcw%3D%3D&amp;btag=e00088000&amp;expire=1735381119&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=9a0a2d2b5655857f30e745893c54ad9b&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/o8OxINivxyq2s8kniJBAEsM8ItzArARCtei9P8/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=1086&amp;bt=543&amp;cs=0&amp;ds=3&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=OWRnOWg0OjYzNGkzOzo2OEBpanZxdnY5cnB0czMzaTczNEBiYWNhMGBhXjYxMWJfNl4uYSMzMGtqMmQ0bWdgLS1kMTJzcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381091&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=3b288d0a2090fb4d7955bfd377738723&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oM2oISfCtDAkCDSG8QFrDRmHpE6g9BqYEsfthE/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=986&amp;bt=493&amp;cs=0&amp;ds=3&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=aWc2ZmQ5ZDk8NTdpOTs5OUBpanhzam85cmVqczMzZzczNEBiLl9iMjNgXjExYi1eNDEwYSNzbmJkMmRjaGRgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381089&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=376e248b454159b006e177ef8d566974&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
     <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/o8F4yPrMvAVrHafIE4ZMSjZCkpefIbDbIY4AQD/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=554&amp;bt=277&amp;cs=0&amp;ds=3&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=Z2ZoODo0NzkzZjM8NmRmZEBpM2c6NnY5cjo5czMzZzczNEAzY2I0L2ExXzYxLzA2XjM1YSNiXzEzMmRzYmNgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381089&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=09b3e929575789998ae62b3df7955055&amp;tk=tt_chain_token</t>
   </si>
   <si>
@@ -274,15 +244,6 @@
     <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oY4Ez9afQBuIkRGChbzDfH0jvJAFgifACgIMIR/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=2480&amp;bt=1240&amp;cs=0&amp;ds=3&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=OGQ2NTU6ZzY6ZzM8M2c5M0BpM2o5ZHE5cmx5cjMzZzczNEA1NC8yYl8uXmIxX2FeYTBhYSNxbjQtMmRjazNgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381090&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=86488f4e008831ad483caad96f850661&amp;tk=tt_chain_token</t>
   </si>
   <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/owERBOIUjDi93vDHBAfmF1AVgbQjgFfdEkamjE/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=1276&amp;bt=638&amp;cs=0&amp;ds=6&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=Ojk5Z2lpNGg8OGc0ZTxpN0Bpams1aWs5cnE3czMzaTczNEAzLWIzY2BhNTUxYzBhMC00YSNtNGhxMmRjYWlgLS1kMTJzcw%3D%3D&amp;btag=e00088000&amp;expire=1735381119&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=9fc1aabfec89d5bcc9e86e2a282b82a9&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/og4nN9AEi2BAMqmieiAypzrs8btiICJ9IxO8Px/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=1054&amp;bt=527&amp;cs=0&amp;ds=6&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=Zzw8OTdkZjU8OjNnaWk4N0BpanZxdnY5cnB0czMzaTczNEAxNTU0NF8tX18xYmFeXjYwYSMzMGtqMmQ0bWdgLS1kMTJzcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381091&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=38bfbef46b0ed56d69cc343b7e4e066f&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
-    <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oIkGefbdIlrNIjLAM77AZCheERWjCbIwhQHBH1/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=942&amp;bt=471&amp;cs=0&amp;ds=6&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=O2gzPDdoNWU7ZTk1Nmc2ZkBpanhzam85cmVqczMzZzczNEBjMy1iYi1gXzExNi80LV9fYSNzbmJkMmRjaGRgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381089&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=2270057513d707e62909cf112858b14f&amp;tk=tt_chain_token</t>
-  </si>
-  <si>
     <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oEIDMvK46DfMIC4YWZ4HzrWAEqkyeanQZAfFjZ/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=714&amp;bt=357&amp;cs=0&amp;ds=6&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=NTQ4aGczaDc1OzRpZ2Y7OkBpM2c6NnY5cjo5czMzZzczNEAvMC80Ni41XjExYGAuYy1fYSNiXzEzMmRzYmNgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381089&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=8b32061a652c51eb1616055bfcb73a1a&amp;tk=tt_chain_token</t>
   </si>
   <si>
@@ -328,15 +289,6 @@
     <t>https://v16-webapp-prime.tiktok.com/video/tos/maliva/tos-maliva-ve-0068c799-us/oUfhAQ4fMeNAwA98bARboee4HHAMiKWTQFycOq/?a=1988&amp;bti=ODszNWYuMDE6&amp;ch=0&amp;cr=3&amp;dr=0&amp;lr=all&amp;cd=0%7C0%7C0%7C&amp;cv=1&amp;br=1940&amp;bt=970&amp;cs=0&amp;ds=6&amp;ft=I~da4ojBD12NvXHU5eIxRMvNglBF-UjNSkopiX&amp;mime_type=video_mp4&amp;qs=0&amp;rc=NGZlaWlpPGk5NTM0NzNoPEBpM2o5ZHE5cmx5cjMzZzczNEAwXzYzXmM2Nl8xMjEwMS9eYSNxbjQtMmRjazNgLS1kMS9zcw%3D%3D&amp;btag=e000b0000&amp;expire=1735381090&amp;l=20241226101800690F34DEA194951EFF21&amp;ply_type=2&amp;policy=2&amp;signature=dc8334150609c76cf1e3af2d2a4a964a&amp;tk=tt_chain_token</t>
   </si>
   <si>
-    <t>https://p16-sign.tiktokcdn-us.com/obj/tos-useast8-p-0068-tx2/ooqHjeKERQ1AvV6fjFID9BDmbImFEEdkBAHbRa?lk3s=81f88b70&amp;x-expires=1735380000&amp;x-signature=Y2rINoZBqgpNgwIDDoIdEG%2F1%2FeQ%3D&amp;shp=81f88b70&amp;shcp=-</t>
-  </si>
-  <si>
-    <t>https://p16-sign.tiktokcdn-us.com/obj/tos-useast8-p-0068-tx2/owVDaeN6EVDCQOFAmN4A7r6fbz5RBYEZnIExlj?lk3s=81f88b70&amp;x-expires=1735380000&amp;x-signature=n5DSyLn0Xv98hbZsZyC5rZw7Puk%3D&amp;shp=81f88b70&amp;shcp=-</t>
-  </si>
-  <si>
-    <t>https://p16-sign.tiktokcdn-us.com/obj/tos-useast5-p-0068-tx/osDmYBD6EDBEshrGfEAgIgEFsQhtLf9oj6CRSC?lk3s=81f88b70&amp;x-expires=1735380000&amp;x-signature=hI0iSnEgXI8fLaFB%2FAE8oRogKo8%3D&amp;shp=81f88b70&amp;shcp=-</t>
-  </si>
-  <si>
     <t>https://p16-sign.tiktokcdn-us.com/obj/tos-useast5-p-0068-tx/oAFAZaZfAY4IM4kMjG4CHrDAyEQMICFeNaMvfD?lk3s=81f88b70&amp;x-expires=1735380000&amp;x-signature=rmTS6Q1n446sNe9LU5dlxePrPYY%3D&amp;shp=81f88b70&amp;shcp=-</t>
   </si>
   <si>
@@ -380,25 +332,16 @@
   </si>
   <si>
     <t>https://p16-sign.tiktokcdn-us.com/obj/tos-useast5-p-0068-tx/o0AGkIJQDzwvfC9hAEfeALCFaFBRuMHIDu0jHb?lk3s=81f88b70&amp;x-expires=1735380000&amp;x-signature=BQp6k1Su4M4Ot7NNy6qJmY6xAfs%3D&amp;shp=81f88b70&amp;shcp=-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What would you like to do this week? Well, this week is Teacher Appreciation Week, so my mom says I have to find something to show my teacher how much I appreciate her. That's a great idea. Teachers work really hard, and it's important to show them how much we appreciate them. You could make a card or a drawing for your teacher. What do you think your teacher would like? I think I'm going to do a drawing for her, because she always likes it when our class draws her things. That's a great idea. I'm sure your teacher will love the drawing. What's your favorite thing about your teacher?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Let's change the subject! Cause we don't have time to unpack all of that!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I cry a lot, but I am so productive. It's an art.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,6 +418,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -521,7 +472,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,9 +504,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,6 +556,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -762,14 +749,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,774 +802,640 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2">
-        <v>45456.04887731482</v>
+        <v>45447.041863425933</v>
       </c>
       <c r="E2">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>11900</v>
+        <v>7715</v>
       </c>
       <c r="G2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2">
-        <v>45454.07523148148</v>
+        <v>45442.049224537041</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>138</v>
       </c>
       <c r="F3">
-        <v>7537</v>
+        <v>8725</v>
       </c>
       <c r="G3">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2">
-        <v>45449.0421412037</v>
+        <v>45435.049837962957</v>
       </c>
       <c r="E4">
+        <v>94</v>
+      </c>
+      <c r="F4">
+        <v>8344</v>
+      </c>
+      <c r="G4">
+        <v>173</v>
+      </c>
+      <c r="H4">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>7994</v>
-      </c>
-      <c r="G4">
-        <v>104</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
       <c r="I4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2">
-        <v>45447.04186342593</v>
+        <v>45433.055891203701</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>7715</v>
+        <v>6037</v>
       </c>
       <c r="G5">
-        <v>209</v>
+        <v>125</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
-        <v>45442.04922453704</v>
+        <v>45428.044270833343</v>
       </c>
       <c r="E6">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F6">
-        <v>8725</v>
+        <v>6157</v>
       </c>
       <c r="G6">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
-        <v>45435.04983796296</v>
+        <v>45426.046377314808</v>
       </c>
       <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>5355</v>
+      </c>
+      <c r="G7">
+        <v>104</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F7">
-        <v>8344</v>
-      </c>
-      <c r="G7">
-        <v>173</v>
-      </c>
-      <c r="H7">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2">
-        <v>45433.0558912037</v>
+        <v>45421.02921296296</v>
       </c>
       <c r="E8">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F8">
-        <v>6037</v>
+        <v>13700</v>
       </c>
       <c r="G8">
-        <v>125</v>
+        <v>546</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2">
-        <v>45428.04427083334</v>
+        <v>45419.004201388889</v>
       </c>
       <c r="E9">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="F9">
-        <v>6157</v>
+        <v>13300</v>
       </c>
       <c r="G9">
-        <v>134</v>
+        <v>339</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
-        <v>45426.04637731481</v>
+        <v>45412.042453703703</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F10">
-        <v>5355</v>
+        <v>7958</v>
       </c>
       <c r="G10">
-        <v>104</v>
+        <v>198</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2">
-        <v>45421.02921296296</v>
+        <v>45407.06454861111</v>
       </c>
       <c r="E11">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="F11">
-        <v>13700</v>
+        <v>8671</v>
       </c>
       <c r="G11">
-        <v>546</v>
+        <v>284</v>
       </c>
       <c r="H11">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I11">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2">
-        <v>45419.00420138889</v>
+        <v>45405.051504629628</v>
       </c>
       <c r="E12">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F12">
-        <v>13300</v>
+        <v>7912</v>
       </c>
       <c r="G12">
-        <v>339</v>
+        <v>236</v>
       </c>
       <c r="H12">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I12">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2">
-        <v>45412.0424537037</v>
+        <v>45398.046273148153</v>
       </c>
       <c r="E13">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>7958</v>
+        <v>11900</v>
       </c>
       <c r="G13">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2">
-        <v>45407.06454861111</v>
+        <v>45391.0469212963</v>
       </c>
       <c r="E14">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F14">
-        <v>8671</v>
+        <v>20100</v>
       </c>
       <c r="G14">
-        <v>284</v>
+        <v>238</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2">
-        <v>45405.05150462963</v>
+        <v>45387.700868055559</v>
       </c>
       <c r="E15">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="F15">
-        <v>7912</v>
+        <v>67500</v>
       </c>
       <c r="G15">
-        <v>236</v>
+        <v>1462</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="I15">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2">
-        <v>45398.04627314815</v>
+        <v>45386.042627314811</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>11900</v>
+        <v>16600</v>
       </c>
       <c r="G16">
-        <v>222</v>
+        <v>280</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45391.0469212963</v>
-      </c>
-      <c r="E17">
-        <v>60</v>
-      </c>
-      <c r="F17">
-        <v>20100</v>
-      </c>
-      <c r="G17">
-        <v>238</v>
-      </c>
-      <c r="H17">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <v>20</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="2">
-        <v>45387.70086805556</v>
-      </c>
-      <c r="E18">
-        <v>95</v>
-      </c>
-      <c r="F18">
-        <v>67500</v>
-      </c>
-      <c r="G18">
-        <v>1462</v>
-      </c>
-      <c r="H18">
-        <v>38</v>
-      </c>
-      <c r="I18">
-        <v>101</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45386.04262731481</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>16600</v>
-      </c>
-      <c r="G19">
-        <v>280</v>
-      </c>
-      <c r="H19">
-        <v>4</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
-    <hyperlink ref="L2" r:id="rId3"/>
-    <hyperlink ref="M2" r:id="rId4"/>
-    <hyperlink ref="J3" r:id="rId5"/>
-    <hyperlink ref="K3" r:id="rId6"/>
-    <hyperlink ref="L3" r:id="rId7"/>
-    <hyperlink ref="M3" r:id="rId8"/>
-    <hyperlink ref="J4" r:id="rId9"/>
-    <hyperlink ref="K4" r:id="rId10"/>
-    <hyperlink ref="L4" r:id="rId11"/>
-    <hyperlink ref="M4" r:id="rId12"/>
-    <hyperlink ref="J5" r:id="rId13"/>
-    <hyperlink ref="K5" r:id="rId14"/>
-    <hyperlink ref="L5" r:id="rId15"/>
-    <hyperlink ref="M5" r:id="rId16"/>
-    <hyperlink ref="J6" r:id="rId17"/>
-    <hyperlink ref="K6" r:id="rId18"/>
-    <hyperlink ref="L6" r:id="rId19"/>
-    <hyperlink ref="M6" r:id="rId20"/>
-    <hyperlink ref="J7" r:id="rId21"/>
-    <hyperlink ref="K7" r:id="rId22"/>
-    <hyperlink ref="L7" r:id="rId23"/>
-    <hyperlink ref="M7" r:id="rId24"/>
-    <hyperlink ref="J8" r:id="rId25"/>
-    <hyperlink ref="K8" r:id="rId26"/>
-    <hyperlink ref="L8" r:id="rId27"/>
-    <hyperlink ref="M8" r:id="rId28"/>
-    <hyperlink ref="J9" r:id="rId29"/>
-    <hyperlink ref="K9" r:id="rId30"/>
-    <hyperlink ref="L9" r:id="rId31"/>
-    <hyperlink ref="M9" r:id="rId32"/>
-    <hyperlink ref="J10" r:id="rId33"/>
-    <hyperlink ref="K10" r:id="rId34"/>
-    <hyperlink ref="L10" r:id="rId35"/>
-    <hyperlink ref="M10" r:id="rId36"/>
-    <hyperlink ref="J11" r:id="rId37"/>
-    <hyperlink ref="K11" r:id="rId38"/>
-    <hyperlink ref="L11" r:id="rId39"/>
-    <hyperlink ref="M11" r:id="rId40"/>
-    <hyperlink ref="J12" r:id="rId41"/>
-    <hyperlink ref="K12" r:id="rId42"/>
-    <hyperlink ref="L12" r:id="rId43"/>
-    <hyperlink ref="M12" r:id="rId44"/>
-    <hyperlink ref="J13" r:id="rId45"/>
-    <hyperlink ref="K13" r:id="rId46"/>
-    <hyperlink ref="L13" r:id="rId47"/>
-    <hyperlink ref="M13" r:id="rId48"/>
-    <hyperlink ref="J14" r:id="rId49"/>
-    <hyperlink ref="K14" r:id="rId50"/>
-    <hyperlink ref="L14" r:id="rId51"/>
-    <hyperlink ref="M14" r:id="rId52"/>
-    <hyperlink ref="J15" r:id="rId53"/>
-    <hyperlink ref="K15" r:id="rId54"/>
-    <hyperlink ref="L15" r:id="rId55"/>
-    <hyperlink ref="M15" r:id="rId56"/>
-    <hyperlink ref="J16" r:id="rId57"/>
-    <hyperlink ref="K16" r:id="rId58"/>
-    <hyperlink ref="L16" r:id="rId59"/>
-    <hyperlink ref="M16" r:id="rId60"/>
-    <hyperlink ref="J17" r:id="rId61"/>
-    <hyperlink ref="K17" r:id="rId62"/>
-    <hyperlink ref="L17" r:id="rId63"/>
-    <hyperlink ref="M17" r:id="rId64"/>
-    <hyperlink ref="J18" r:id="rId65"/>
-    <hyperlink ref="K18" r:id="rId66"/>
-    <hyperlink ref="L18" r:id="rId67"/>
-    <hyperlink ref="M18" r:id="rId68"/>
-    <hyperlink ref="J19" r:id="rId69"/>
-    <hyperlink ref="K19" r:id="rId70"/>
-    <hyperlink ref="L19" r:id="rId71"/>
-    <hyperlink ref="M19" r:id="rId72"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="K3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="K4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L5" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K6" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="J7" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="K7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M7" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="J8" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="K8" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L8" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M8" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="J9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="K9" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L9" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="M9" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="J10" r:id="rId33" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="K10" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L10" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="M10" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="J11" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="K11" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="L11" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="M11" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="J12" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="K12" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L12" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="M12" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="J13" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="K13" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L13" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="M13" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="J14" r:id="rId49" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="K14" r:id="rId50" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="L14" r:id="rId51" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="M14" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J15" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="K15" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L15" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="M15" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="J16" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="K16" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L16" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="M16" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId61"/>
 </worksheet>
 </file>
</xml_diff>